<commit_message>
Status Update - (07-05-2020)
</commit_message>
<xml_diff>
--- a/REVER_DailyTracker_20200505.xlsx
+++ b/REVER_DailyTracker_20200505.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\DailyTracker-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478737AD-C083-45C4-8C16-45E441CB0020}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D54BC3C-20E1-486A-9205-0295B8537F68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{BDBCA639-774E-4870-AA16-72178DF9137C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>RPA-SALE</t>
-  </si>
-  <si>
-    <t>Video Management - Create,view,update,delete</t>
   </si>
   <si>
     <t>PPT Management - Create,view,update,delete</t>
@@ -1301,7 +1298,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1352,7 +1349,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="24">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>3</v>
@@ -1370,13 +1367,13 @@
         <v>18</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="24">
-        <v>0.9</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="G3" s="21"/>
     </row>
@@ -1391,7 +1388,7 @@
         <v>18</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="24">
         <v>0.8</v>
@@ -1401,7 +1398,27 @@
       </c>
       <c r="G4" s="21"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1"/>
+    <row r="5" spans="1:7" s="4" customFormat="1">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="23">
+        <v>43958</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="24">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="21"/>
+    </row>
     <row r="6" spans="1:7" s="4" customFormat="1"/>
     <row r="7" spans="1:7" s="4" customFormat="1"/>
     <row r="8" spans="1:7" s="4" customFormat="1"/>

</xml_diff>